<commit_message>
vault backup: 2022-12-02 10:19:49
Affected files:
Scite/scite kuer/groupe sanguins/2. Hérédité des groupes sanguins.docx
Scite/scite kuer/groupe sanguins/3. Phénotype et génotype groupes sanguins.xlsx
Scite/scite kuer/groupe sanguins/~$ Hérédité des groupes sanguins.docx
Scite/scite kuer/groupe sanguins/~$3. Phénotype et génotype groupes sanguins.xlsx
</commit_message>
<xml_diff>
--- a/Scite/scite kuer/groupe sanguins/3. Phénotype et génotype groupes sanguins.xlsx
+++ b/Scite/scite kuer/groupe sanguins/3. Phénotype et génotype groupes sanguins.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09460399-E0D9-4734-9063-E9021FB3F226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lousergonne/Documents/GitHub/obsidian/Scite/scite kuer/groupe sanguins/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47FACBB-FCED-8F42-BE48-7B21AC3D68DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,7 +291,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,7 +656,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -939,7 +944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -949,16 +954,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="190" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C3" s="6"/>
       <c r="D3" s="1"/>
       <c r="E3" s="57" t="s">
@@ -976,7 +981,7 @@
       <c r="O3" s="57"/>
       <c r="P3" s="58"/>
     </row>
-    <row r="4" spans="3:16">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C4" s="5"/>
       <c r="D4" s="17"/>
       <c r="E4" s="12" t="s">
@@ -1004,7 +1009,7 @@
       </c>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="3:16">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C5" s="59" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1046,7 @@
       </c>
       <c r="P5" s="20"/>
     </row>
-    <row r="6" spans="3:16">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C6" s="59"/>
       <c r="D6" s="8"/>
       <c r="E6" s="2"/>
@@ -1057,7 +1062,7 @@
       <c r="O6" s="21"/>
       <c r="P6" s="22"/>
     </row>
-    <row r="7" spans="3:16">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C7" s="59"/>
       <c r="D7" s="9" t="s">
         <v>2</v>
@@ -1099,7 +1104,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="3:16">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C8" s="59"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
@@ -1127,7 +1132,7 @@
       <c r="O8" s="19"/>
       <c r="P8" s="20"/>
     </row>
-    <row r="9" spans="3:16">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C9" s="59"/>
       <c r="D9" s="7" t="s">
         <v>3</v>
@@ -1169,7 +1174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:16">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C10" s="59"/>
       <c r="D10" s="8"/>
       <c r="E10" s="15"/>
@@ -1197,7 +1202,7 @@
       <c r="O10" s="21"/>
       <c r="P10" s="22"/>
     </row>
-    <row r="11" spans="3:16">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C11" s="59"/>
       <c r="D11" s="9" t="s">
         <v>4</v>
@@ -1239,7 +1244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="3:16">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C12" s="59"/>
       <c r="D12" s="9"/>
       <c r="E12" s="3"/>
@@ -1267,7 +1272,7 @@
       <c r="O12" s="19"/>
       <c r="P12" s="20"/>
     </row>
-    <row r="13" spans="3:16">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C13" s="59"/>
       <c r="D13" s="7" t="s">
         <v>5</v>
@@ -1303,7 +1308,7 @@
       </c>
       <c r="P13" s="23"/>
     </row>
-    <row r="14" spans="3:16">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C14" s="59"/>
       <c r="D14" s="8"/>
       <c r="E14" s="15"/>
@@ -1319,7 +1324,7 @@
       <c r="O14" s="21"/>
       <c r="P14" s="22"/>
     </row>
-    <row r="15" spans="3:16">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C15" s="59"/>
       <c r="D15" s="9" t="s">
         <v>6</v>
@@ -1355,7 +1360,7 @@
       </c>
       <c r="P15" s="20"/>
     </row>
-    <row r="16" spans="3:16">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C16" s="60"/>
       <c r="D16" s="10"/>
       <c r="E16" s="2"/>
@@ -1371,22 +1376,22 @@
       <c r="O16" s="21"/>
       <c r="P16" s="22"/>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="29" t="s">
         <v>23</v>
       </c>
@@ -1401,6 +1406,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ffc58c69-6c74-4308-be08-94fe657bd9ff">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d6c1408c-acd5-4d01-b1b2-7dd1b1dc95e2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B8CCF3A4CC2B849851D1D2DA8EA8C63" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4b26649ea5378df9af31742c04143ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffc58c69-6c74-4308-be08-94fe657bd9ff" xmlns:ns3="d6c1408c-acd5-4d01-b1b2-7dd1b1dc95e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="75fbcc99cbd78acfaef083e99f930be6" ns2:_="" ns3:_="">
     <xsd:import namespace="ffc58c69-6c74-4308-be08-94fe657bd9ff"/>
@@ -1611,34 +1636,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ffc58c69-6c74-4308-be08-94fe657bd9ff">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d6c1408c-acd5-4d01-b1b2-7dd1b1dc95e2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF552B6-0276-4AA2-9D88-3B9F3E42E758}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B091E98B-B935-4EDF-9ED5-8AE8185AFE9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ffc58c69-6c74-4308-be08-94fe657bd9ff"/>
+    <ds:schemaRef ds:uri="d6c1408c-acd5-4d01-b1b2-7dd1b1dc95e2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A13943F0-AE0C-472B-B889-D4FE867432A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A13943F0-AE0C-472B-B889-D4FE867432A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B091E98B-B935-4EDF-9ED5-8AE8185AFE9A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF552B6-0276-4AA2-9D88-3B9F3E42E758}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ffc58c69-6c74-4308-be08-94fe657bd9ff"/>
+    <ds:schemaRef ds:uri="d6c1408c-acd5-4d01-b1b2-7dd1b1dc95e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>